<commit_message>
updated instructions for widefield
</commit_message>
<xml_diff>
--- a/templates/input_widefield_2P.xlsx
+++ b/templates/input_widefield_2P.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\nwb\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Jacob\nwb_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D69B4FE2-F37F-4131-94B6-3A27E2D190FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7F8EB-0132-448E-917D-98B71DB2D5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31995" yWindow="5535" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="auto" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="113">
   <si>
     <t>session_id</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>Fig 4b, 4c, 4d, 4e, 4f, 5c, 6b, 6c, 6d, 6e, 6f, S7a, S7b, S7c, S6c, S8a, S8b, S8c</t>
+  </si>
+  <si>
+    <t>Z:\Jacob\nwb_process\recordings\M4_recordings.xlsx</t>
   </si>
 </sst>
 </file>
@@ -868,9 +871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG13" sqref="AG13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,6 +2313,9 @@
       <c r="K27" s="4" t="s">
         <v>111</v>
       </c>
+      <c r="L27" t="s">
+        <v>112</v>
+      </c>
       <c r="M27" t="s">
         <v>77</v>
       </c>

</xml_diff>